<commit_message>
change on preview excel
</commit_message>
<xml_diff>
--- a/outputs/11_output.xlsx
+++ b/outputs/11_output.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -204,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -270,6 +270,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,7 +353,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>11</col>
@@ -362,21 +368,21 @@
         <cNvPicPr preferRelativeResize="0"/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="7513320" y="137160"/>
           <a:ext cx="2095500" cy="523875"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -687,7 +693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -717,19 +723,26 @@
       </c>
     </row>
     <row r="2" ht="18" customHeight="1">
-      <c r="B2" s="1" t="inlineStr">
+      <c r="A2" s="29" t="n"/>
+      <c r="B2" s="30" t="inlineStr">
         <is>
           <t>MASTERFILE EQUIPMENT</t>
         </is>
       </c>
+      <c r="C2" s="29" t="n"/>
+      <c r="D2" s="29" t="n"/>
     </row>
     <row r="3" ht="18" customHeight="1">
-      <c r="B3" s="1" t="inlineStr">
+      <c r="A3" s="29" t="n"/>
+      <c r="B3" s="30" t="inlineStr">
         <is>
           <t>TOTAL NO. OF EQUIPMENT: 10 EQUIPMENTS</t>
         </is>
       </c>
-    </row>
+      <c r="C3" s="29" t="n"/>
+      <c r="D3" s="29" t="n"/>
+    </row>
+    <row r="4"/>
     <row r="5">
       <c r="A5" s="19" t="inlineStr">
         <is>
@@ -854,36 +867,35 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="29" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="29" t="inlineStr">
         <is>
           <t>V-001</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="29" t="inlineStr">
         <is>
           <t>MLK_PMT_10102_-_V-002</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" s="29" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>PLATE 1571x600x5mm SHELL TO BE ROLLED</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>Shell Plate</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>DMSD</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Stainless Steel</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -923,41 +935,24 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>DISH HEAD 8Thk TO BE FORMED T.D 2:1 TYPE</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>Dish Head</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>DMSD</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Stainless Steel</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>SA-240M</t>
+          <t>SA-240</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -992,46 +987,29 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>SEAMLESS PIPE DN50 x 87 SCH 40s</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
+          <t>Seamless Pipe DN50</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>DMSD</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Stainless Steel</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>SA-312M</t>
+          <t>SA-312</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>TP316L</t>
+          <t>TP 316L</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1061,46 +1039,29 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>SEAMLESS PIPE DN25 x 100 SCH 40s</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>Seamless Pipe DN25</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>DMSD</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Stainless Steel</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>SA-312M</t>
+          <t>SA-312</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>TP316L</t>
+          <t>TP 316L</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1130,46 +1091,29 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>SEAMLESS PIPE DN50 x 112 SCH 40s</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
+          <t>Seamless Pipe DN50</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>DMSD</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Stainless Steel</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>SA-312M</t>
+          <t>SA-312</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>TP316L</t>
+          <t>TP 316L</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1199,570 +1143,546 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>FLANGE DN50 CLASS 150 WNRF SCH 40s</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
+          <t>Seamless Pipe DN50</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>DMSD</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Stainless Steel</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
+          <t>SA-312</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>TP 316L</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>1.1 BarG</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>1.0 BarG</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Flange DN50 Class 150 WNRF</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>DMSD</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
           <t>SA-182</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>F316L</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
         <is>
           <t>1.1 BarG</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>1.0 BarG</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>FLANGE DN50 CLASS 150 WNRF SCH 40s</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>DMSO</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
+    <row r="15">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Flange DN25 Class 150 WNRF</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>DMSD</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>SA-182</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>F316L</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
         <is>
           <t>1.1 BarG</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
         <is>
           <t>1.0 BarG</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>FLANGE DN25 CLASS 150 WNRF SCH 40s</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>DMSO</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
+    <row r="16">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Flange DN50 Class 150 WNRF</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>DMSD</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>SA-182</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>F316L</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t>1.1 BarG</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
         <is>
           <t>1.0 BarG</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>BASE PLATE 150 x 150 x 5Thk</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>DMSO</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
+    <row r="17">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Flange DN50 Class 150 WNRF</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>DMSD</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>SA-182</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>F316L</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>1.1 BarG</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>1.0 BarG</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Base Plate</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>DMSD</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>SA-240</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Gr.304</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Gr 304</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
         <is>
           <t>1.1 BarG</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
         <is>
           <t>1.0 BarG</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>LIFTING LUG PLATE 190 x 80 x 6Thk</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>DMSO</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
+    <row r="19">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Lifting Lug Plate</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>DMSD</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>SA-240</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Gr.304</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>316L</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
         <is>
           <t>1.1 BarG</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
         <is>
           <t>1.0 BarG</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>DOUBLER PLATE 120 x 150 x 12.7Thk</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>DMSO</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
+    <row r="20">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Doubler Plate</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>DMSD</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>SA-240</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Gr.304</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>316L</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
         <is>
           <t>1.1 BarG</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
         <is>
           <t>1.0 BarG</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>EQUAL ANGLE BAR 3" x 3" x 1/4" Thk</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>DMSO</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
+    <row r="21">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Equal Angle Bar</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>DMSD</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>SA-240</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>Gr.304</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Gr 304</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
         <is>
           <t>1.1 BarG</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
         <is>
           <t>1.0 BarG</t>
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>V-001</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>MLK_PMT_10102_-_V-002</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>EARTHING LUG</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>DMSO</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Earthing Lug</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>DMSD</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>SA-240</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Gr.304</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Gr 304</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
         <is>
           <t>1.1 BarG</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>100 °C</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
         <is>
           <t>1.0 BarG</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="19">
     <mergeCell ref="D5:D7"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="H5:J6"/>
-    <mergeCell ref="C5:C7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="G5:G7"/>
+    <mergeCell ref="B8:B22"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C8:C22"/>
+    <mergeCell ref="C5:C7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="K5:K7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="A8:A22"/>
+    <mergeCell ref="D8:D22"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="L5:M6"/>
-    <mergeCell ref="F5:F7"/>
     <mergeCell ref="N5:O6"/>
-    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>